<commit_message>
Ajuste en solicitud gráfica
LE_06_05_REC360
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion05/LE_06_05_REC360_SolicitudGrafica.xlsx
+++ b/fuentes/contenidos/grado06/guion05/LE_06_05_REC360_SolicitudGrafica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\PLANETA\NUEVO\GUIONES\LE_06_05_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\GitHub\Lenguaje\fuentes\contenidos\grado06\guion05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="201">
   <si>
     <t>Fecha:</t>
   </si>
@@ -609,6 +609,27 @@
   </si>
   <si>
     <t xml:space="preserve">hombre entrevista a mujer </t>
+  </si>
+  <si>
+    <t>MUJER ENTREVISTANDO A UN HOMBRE</t>
+  </si>
+  <si>
+    <t>SÍMBOLOS RELACIONADOS CON EL PERIODISMO</t>
+  </si>
+  <si>
+    <t>HOMBRE MIRANDO DIBUJO DEL MUNDO</t>
+  </si>
+  <si>
+    <t>HOMBRE ESTUDIANDO</t>
+  </si>
+  <si>
+    <t>MUJER PENSANDO EN ESCRIBIR</t>
+  </si>
+  <si>
+    <t>ALGUIEN MARCANDO UNA FECHA EN EL CALENDARIO</t>
+  </si>
+  <si>
+    <t>ALGUIEN ESCRIBIENDO</t>
   </si>
 </sst>
 </file>
@@ -1556,6 +1577,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1654,7 +1676,6 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2491,9 +2512,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2539,14 +2560,14 @@
       <c r="B2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="86"/>
-      <c r="F2" s="78" t="s">
+      <c r="D2" s="87"/>
+      <c r="F2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="79"/>
+      <c r="G2" s="80"/>
       <c r="H2" s="58"/>
       <c r="I2" s="58"/>
       <c r="J2" s="14"/>
@@ -2570,14 +2591,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="87">
+      <c r="C3" s="88">
         <v>6</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="F3" s="80">
+      <c r="D3" s="89"/>
+      <c r="F3" s="81">
         <v>42412</v>
       </c>
-      <c r="G3" s="81"/>
+      <c r="G3" s="82"/>
       <c r="H3" s="58"/>
       <c r="I3" s="38"/>
       <c r="J3" s="14"/>
@@ -2601,10 +2622,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="88" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="88"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="5"/>
       <c r="F4" s="37" t="s">
         <v>55</v>
@@ -2633,10 +2654,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="90"/>
+      <c r="D5" s="91"/>
       <c r="E5" s="5"/>
       <c r="F5" s="37" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2720,12 +2741,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="85"/>
       <c r="J8" s="16"/>
       <c r="K8" s="11"/>
       <c r="M8" s="2" t="str">
@@ -2786,7 +2807,7 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="109">
+      <c r="B10" s="78">
         <v>154948568</v>
       </c>
       <c r="C10" s="20" t="str">
@@ -2829,7 +2850,7 @@
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="109">
+      <c r="B11" s="78">
         <v>332871782</v>
       </c>
       <c r="C11" s="20" t="str">
@@ -2872,7 +2893,7 @@
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="109">
+      <c r="B12" s="78">
         <v>173622302</v>
       </c>
       <c r="C12" s="20" t="str">
@@ -2910,25 +2931,31 @@
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B13" s="62"/>
+        <v>IMG04</v>
+      </c>
+      <c r="B13" s="78">
+        <v>262339847</v>
+      </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
+        <v>Recurso F13B</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>168</v>
+      </c>
       <c r="F13" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>LE_06_05_REC360_IMG04.jpg</v>
       </c>
       <c r="G13" s="13" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>270 x 375 px</v>
       </c>
       <c r="H13" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -2938,32 +2965,40 @@
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J13" s="64"/>
+      <c r="J13" s="64" t="s">
+        <v>194</v>
+      </c>
       <c r="K13" s="64"/>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B14" s="62"/>
+        <v>IMG05</v>
+      </c>
+      <c r="B14" s="78">
+        <v>244122844</v>
+      </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
+        <v>Recurso F13B</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>168</v>
+      </c>
       <c r="F14" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>LE_06_05_REC360_IMG05.jpg</v>
       </c>
       <c r="G14" s="13" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>270 x 375 px</v>
       </c>
       <c r="H14" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -2973,32 +3008,40 @@
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J14" s="64"/>
+      <c r="J14" s="64" t="s">
+        <v>195</v>
+      </c>
       <c r="K14" s="64"/>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B15" s="62"/>
+        <v>IMG06</v>
+      </c>
+      <c r="B15" s="78">
+        <v>255673432</v>
+      </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
+        <v>Recurso F13B</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>168</v>
+      </c>
       <c r="F15" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>LE_06_05_REC360_IMG06.jpg</v>
       </c>
       <c r="G15" s="13" t="str">
         <f ca="1">IF($F15&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>270 x 375 px</v>
       </c>
       <c r="H15" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3008,32 +3051,40 @@
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J15" s="66"/>
+      <c r="J15" s="66" t="s">
+        <v>196</v>
+      </c>
       <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B16" s="62"/>
+        <v>IMG07</v>
+      </c>
+      <c r="B16" s="78">
+        <v>217035724</v>
+      </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
+        <v>Recurso F13B</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>168</v>
+      </c>
       <c r="F16" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>LE_06_05_REC360_IMG07.jpg</v>
       </c>
       <c r="G16" s="13" t="str">
         <f ca="1">IF($F16&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>270 x 375 px</v>
       </c>
       <c r="H16" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3043,32 +3094,40 @@
         <f ca="1">IF(OR($B16&lt;&gt;"",$J16&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J16" s="67"/>
+      <c r="J16" s="67" t="s">
+        <v>197</v>
+      </c>
       <c r="K16" s="68"/>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
         <v>F7</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B17" s="62"/>
+        <v>IMG08</v>
+      </c>
+      <c r="B17" s="78">
+        <v>341004944</v>
+      </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
+        <v>Recurso F13B</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>168</v>
+      </c>
       <c r="F17" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>LE_06_05_REC360_IMG08.jpg</v>
       </c>
       <c r="G17" s="13" t="str">
         <f ca="1">IF($F17&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>270 x 375 px</v>
       </c>
       <c r="H17" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3078,32 +3137,40 @@
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J17" s="66"/>
+      <c r="J17" s="66" t="s">
+        <v>198</v>
+      </c>
       <c r="K17" s="66"/>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
         <v>F7B</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B18" s="62"/>
+        <v>IMG09</v>
+      </c>
+      <c r="B18" s="78">
+        <v>262750391</v>
+      </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
+        <v>Recurso F13B</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>168</v>
+      </c>
       <c r="F18" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>LE_06_05_REC360_IMG09.jpg</v>
       </c>
       <c r="G18" s="13" t="str">
         <f ca="1">IF($F18&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>270 x 375 px</v>
       </c>
       <c r="H18" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3113,32 +3180,40 @@
         <f ca="1">IF(OR($B18&lt;&gt;"",$J18&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J18" s="66"/>
+      <c r="J18" s="66" t="s">
+        <v>199</v>
+      </c>
       <c r="K18" s="66"/>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
         <v>F8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
-        <v/>
-      </c>
-      <c r="B19" s="62"/>
+        <v>IMG10</v>
+      </c>
+      <c r="B19" s="78">
+        <v>308524523</v>
+      </c>
       <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
+        <v>Recurso F13B</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19" s="63" t="s">
+        <v>168</v>
+      </c>
       <c r="F19" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>LE_06_05_REC360_IMG10.jpg</v>
       </c>
       <c r="G19" s="13" t="str">
         <f ca="1">IF($F19&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>270 x 375 px</v>
       </c>
       <c r="H19" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3148,7 +3223,9 @@
         <f ca="1">IF(OR($B19&lt;&gt;"",$J19&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J19" s="67"/>
+      <c r="J19" s="67" t="s">
+        <v>200</v>
+      </c>
       <c r="K19" s="68"/>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>
@@ -6004,25 +6081,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="95"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="96"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31"/>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -6030,11 +6107,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
       <c r="F3" s="32"/>
       <c r="H3" s="22" t="s">
         <v>18</v>
@@ -6085,11 +6162,11 @@
       <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="105" t="str">
+      <c r="D5" s="106" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="106"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="32"/>
       <c r="H5" s="22" t="s">
         <v>22</v>
@@ -6134,12 +6211,12 @@
       <c r="C7" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="91" t="str">
+      <c r="D7" s="92" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="93"/>
       <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
@@ -6233,14 +6310,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="95"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="96"/>
       <c r="I13" s="22" t="s">
         <v>33</v>
       </c>
@@ -6273,12 +6350,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="99"/>
       <c r="J15" s="22">
         <v>12</v>
       </c>
@@ -6318,12 +6395,12 @@
       <c r="C17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="99" t="str">
+      <c r="D17" s="100" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="100"/>
-      <c r="F17" s="101"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="102"/>
       <c r="J17" s="22">
         <v>14</v>
       </c>
@@ -6339,12 +6416,12 @@
       <c r="C18" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="91" t="str">
+      <c r="D18" s="92" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="91"/>
-      <c r="F18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="93"/>
       <c r="J18" s="22">
         <v>15</v>
       </c>
@@ -6735,40 +6812,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="109" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="107" t="s">
+      <c r="H1" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="107"/>
+      <c r="I1" s="108"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
+      <c r="A2" s="109"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
       <c r="H2" s="39" t="s">
         <v>65</v>
       </c>

</xml_diff>